<commit_message>
Update Config file (price of fuel/CO2/unserved heat)
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED9A67-3D96-4171-BC6B-03CE78CAF077}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73F6954-4811-4C68-A9C7-A1AEFC770E26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="219">
   <si>
     <t>Default value</t>
   </si>
@@ -585,18 +585,6 @@
   </si>
   <si>
     <t>Active zone</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Coal/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Gas/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Oil/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Biomass/2015.csv</t>
   </si>
   <si>
     <t>Z1</t>
@@ -1405,8 +1393,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1424,7 +1412,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1472,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -1617,7 +1605,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1759,10 +1747,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1770,13 +1758,13 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C62" s="4">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1937,7 +1925,7 @@
         <v>60</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>141</v>
@@ -1979,7 +1967,7 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1993,7 +1981,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2039,7 +2027,7 @@
         <v>36</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>89</v>
@@ -2048,7 +2036,7 @@
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B126" s="29" t="s">
         <v>36</v>
@@ -2061,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="5">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H126" s="11"/>
     </row>
@@ -2073,7 +2061,7 @@
         <v>36</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D127" s="18" t="s">
         <v>89</v>
@@ -2090,13 +2078,13 @@
         <v>36</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>89</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2107,7 +2095,7 @@
         <v>36</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>89</v>
@@ -2128,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="5">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="H130" s="11" t="s">
         <v>70</v>
@@ -2142,7 +2130,7 @@
         <v>36</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>89</v>
@@ -2174,7 +2162,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>89</v>
@@ -2203,7 +2191,7 @@
         <v>36</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>89</v>
@@ -2211,13 +2199,13 @@
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B136" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>89</v>
@@ -2226,13 +2214,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>89</v>
@@ -2332,7 +2320,7 @@
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B161" s="29" t="s">
         <v>36</v>
@@ -2341,7 +2329,7 @@
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="25" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B162" s="29" t="s">
         <v>36</v>
@@ -2350,7 +2338,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="28" t="s">
@@ -2360,12 +2348,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E164" s="28" t="s">
         <v>0</v>
@@ -2374,7 +2362,7 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2383,7 +2371,7 @@
     </row>
     <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="35" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="37"/>
@@ -2408,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="5">
-        <v>7</v>
+        <v>350</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2426,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>50</v>
+        <v>175</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -2452,7 +2440,7 @@
     </row>
     <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>36</v>
@@ -2468,12 +2456,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="26" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>36</v>
@@ -2538,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="F181" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2548,9 +2536,7 @@
       <c r="B182" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C182" s="19" t="s">
-        <v>184</v>
-      </c>
+      <c r="C182" s="19"/>
       <c r="D182" s="18" t="s">
         <v>89</v>
       </c>
@@ -2558,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="F182" s="5">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2568,9 +2554,7 @@
       <c r="B183" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C183" s="19" t="s">
-        <v>185</v>
-      </c>
+      <c r="C183" s="19"/>
       <c r="D183" s="18" t="s">
         <v>89</v>
       </c>
@@ -2578,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="F183" s="5">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="H183" s="1" t="s">
         <v>125</v>
@@ -2591,9 +2575,7 @@
       <c r="B184" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C184" s="19" t="s">
-        <v>186</v>
-      </c>
+      <c r="C184" s="19"/>
       <c r="D184" s="18" t="s">
         <v>89</v>
       </c>
@@ -2601,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="F184" s="5">
-        <v>35</v>
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2611,9 +2593,7 @@
       <c r="B185" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C185" s="19" t="s">
-        <v>187</v>
-      </c>
+      <c r="C185" s="19"/>
       <c r="D185" s="18" t="s">
         <v>89</v>
       </c>
@@ -2621,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="F185" s="5">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2639,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="F186" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2731,7 +2711,7 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2866,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>0</v>
@@ -2880,13 +2860,13 @@
         <v>52</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D227" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E227" s="6" t="s">
         <v>18</v>
@@ -2895,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="G227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2907,7 +2887,7 @@
         <v>1</v>
       </c>
       <c r="D228" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E228" s="6" t="s">
         <v>19</v>
@@ -2916,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="G228" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2937,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="G229" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2949,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="D230" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E230" s="6" t="s">
         <v>153</v>
@@ -2970,7 +2950,7 @@
         <v>1</v>
       </c>
       <c r="D231" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E231" s="6" t="s">
         <v>154</v>
@@ -3012,7 +2992,7 @@
         <v>1</v>
       </c>
       <c r="D233" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E233" s="6" t="s">
         <v>21</v>
@@ -3042,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="G234" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3054,7 +3034,7 @@
         <v>1</v>
       </c>
       <c r="D235" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E235" s="6" t="s">
         <v>32</v>
@@ -3063,7 +3043,7 @@
         <v>1</v>
       </c>
       <c r="G235" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3075,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="D236" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E236" s="6" t="s">
         <v>23</v>
@@ -3084,7 +3064,7 @@
         <v>1</v>
       </c>
       <c r="G236" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3096,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="D237" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E237" s="6" t="s">
         <v>24</v>
@@ -3105,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="G237" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3117,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="D238" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E238" s="6" t="s">
         <v>25</v>
@@ -3126,7 +3106,7 @@
         <v>1</v>
       </c>
       <c r="G238" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3138,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="D239" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E239" s="6" t="s">
         <v>157</v>
@@ -3159,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="D240" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E240" s="6" t="s">
         <v>158</v>
@@ -3180,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="D241" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E241" s="6" t="s">
         <v>29</v>
@@ -3189,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="G241" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3200,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="D242" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E242" s="6" t="s">
         <v>26</v>
@@ -3209,7 +3189,7 @@
         <v>1</v>
       </c>
       <c r="G242" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3220,7 +3200,7 @@
         <v>1</v>
       </c>
       <c r="D243" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E243" s="6" t="s">
         <v>27</v>
@@ -3229,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="G243" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3240,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="D244" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E244" s="6" t="s">
         <v>159</v>
@@ -3263,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="D245" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E245" s="6" t="s">
         <v>160</v>
@@ -3293,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="G246" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H246" s="1" t="s">
         <v>139</v>
@@ -3307,7 +3287,7 @@
         <v>1</v>
       </c>
       <c r="D247" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E247" s="6" t="s">
         <v>162</v>
@@ -3652,7 +3632,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A325" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Get ready for simulation
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5846DB1-C664-4A51-A263-30B7CF2E2C04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331C1AE-3D04-4C9F-AD74-18172690F9D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="218">
   <si>
     <t>Default value</t>
   </si>
@@ -657,9 +657,6 @@
   </si>
   <si>
     <t>H2 Demand</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/OutageFactors/##/2016.csv</t>
   </si>
   <si>
     <t>Database/NearZeroCarbon/PowerPlants/##/JRC_EU_TIMES_NearZeroCarbon_2050_ALLFLEX.csv</t>
@@ -1394,7 +1391,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -1605,7 +1602,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -2027,7 +2024,7 @@
         <v>36</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>89</v>
@@ -2060,9 +2057,7 @@
       <c r="B127" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C127" s="23" t="s">
-        <v>208</v>
-      </c>
+      <c r="C127" s="23"/>
       <c r="D127" s="18" t="s">
         <v>89</v>
       </c>
@@ -2078,7 +2073,7 @@
         <v>36</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>89</v>
@@ -2095,7 +2090,7 @@
         <v>36</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>89</v>
@@ -2130,7 +2125,7 @@
         <v>36</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>89</v>
@@ -2162,7 +2157,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>89</v>
@@ -2191,7 +2186,7 @@
         <v>36</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>89</v>
@@ -2205,7 +2200,7 @@
         <v>36</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>89</v>
@@ -2220,7 +2215,7 @@
         <v>36</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Increase water value to have better profiles
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331C1AE-3D04-4C9F-AD74-18172690F9D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE1932-8505-4660-B961-B6C3501E3F32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1390,8 +1390,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>150</v>

</xml_diff>

<commit_message>
Add possibility for PtL H2 demand + MODIFICATION OF CONFIG FILE
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE1932-8505-4660-B961-B6C3501E3F32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979EB48C-7A96-4A23-B6C7-90592591B5B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="223">
   <si>
     <t>Default value</t>
   </si>
@@ -605,9 +605,6 @@
     <t>The path is an absolute path or a relative path to this config file</t>
   </si>
   <si>
-    <t>Dispa-SET Configuration File (v20.01)</t>
-  </si>
-  <si>
     <t>This value imposes the final (relative) reservoir levels if the option is set to true</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
     <t>Number of equivalent storage hours for the flexibile demand</t>
   </si>
   <si>
-    <t>End of the Config file. This must be line number 325!</t>
-  </si>
-  <si>
     <t>Price of Transmission</t>
   </si>
   <si>
@@ -656,9 +650,6 @@
     <t>Price of Unserved H2</t>
   </si>
   <si>
-    <t>H2 Demand</t>
-  </si>
-  <si>
     <t>Database/NearZeroCarbon/PowerPlants/##/JRC_EU_TIMES_NearZeroCarbon_2050_ALLFLEX.csv</t>
   </si>
   <si>
@@ -674,9 +665,6 @@
     <t>Database/NearZeroCarbon/Temperatures/Temperatures_ProRes1_2050.csv</t>
   </si>
   <si>
-    <t>Database/NearZeroCarbon/H2_demand/H2_demand_2050.csv</t>
-  </si>
-  <si>
     <t>Database/NearZeroCarbon/TotalLoadValue/##/1h/TotalLoadValue_NearZeroCarbon_2050.csv</t>
   </si>
   <si>
@@ -687,6 +675,33 @@
   </si>
   <si>
     <t>Database/NearZeroCarbon/DayAheadNTC/1h/NTC_2050.csv</t>
+  </si>
+  <si>
+    <t>H2 rigid Demand</t>
+  </si>
+  <si>
+    <t>H2 flexible demand</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/H2_rigid_Demand_2050.csv</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/H2_PtL_Demand_2050.csv</t>
+  </si>
+  <si>
+    <t>H2 flexible capacities</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities.csv</t>
+  </si>
+  <si>
+    <t>Can remain empty if no flexible part of the H2 demand</t>
+  </si>
+  <si>
+    <t>End of the Config file. This must be line number 327!</t>
+  </si>
+  <si>
+    <t>Dispa-SET Configuration File (v20.02)</t>
   </si>
 </sst>
 </file>
@@ -847,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -981,6 +996,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1048,9 +1069,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFACC0AC"/>
       <color rgb="FFE9D7A6"/>
       <color rgb="FFA1A295"/>
-      <color rgb="FFACC0AC"/>
       <color rgb="FFECBE8B"/>
       <color rgb="FFD9AE8F"/>
     </mruColors>
@@ -1388,10 +1409,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="F207" sqref="F207"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="F182" sqref="F182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1408,16 +1429,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1432,15 +1453,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
@@ -1456,15 +1477,15 @@
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="B6" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="45"/>
@@ -1602,7 +1623,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1744,10 +1765,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1755,10 +1776,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>196</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1964,7 +1985,7 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1978,7 +1999,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2024,7 +2045,7 @@
         <v>36</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>89</v>
@@ -2073,7 +2094,7 @@
         <v>36</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>89</v>
@@ -2090,7 +2111,7 @@
         <v>36</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>89</v>
@@ -2125,7 +2146,7 @@
         <v>36</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>89</v>
@@ -2157,7 +2178,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>89</v>
@@ -2186,7 +2207,7 @@
         <v>36</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>89</v>
@@ -2200,7 +2221,7 @@
         <v>36</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>89</v>
@@ -2209,13 +2230,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>89</v>
@@ -2249,172 +2270,164 @@
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="25"/>
-      <c r="C160" s="27"/>
-    </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B160" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C160" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="H160" s="26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="B161" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="B161" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C161" s="19"/>
-    </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="B162" s="29" t="s">
+      <c r="C161" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="H161" s="26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="25"/>
+      <c r="C162" s="27"/>
+    </row>
+    <row r="163" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B163" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C162" s="19"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A163" s="2" t="s">
+      <c r="C163" s="19"/>
+    </row>
+    <row r="164" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B164" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C164" s="19"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A165" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C165" s="1"/>
+      <c r="E165" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F165" s="5">
+        <v>4</v>
+      </c>
+      <c r="H165" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C163" s="1"/>
-      <c r="E163" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F163" s="5">
-        <v>4</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A164" s="2" t="s">
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A166" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E166" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F166" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H166" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E164" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F164" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="H164" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="25"/>
-      <c r="C165" s="27"/>
-    </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="35" t="s">
+    </row>
+    <row r="167" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="25"/>
+      <c r="C167" s="27"/>
+    </row>
+    <row r="168" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B166" s="36"/>
-      <c r="C166" s="37"/>
-      <c r="D166" s="36"/>
-      <c r="E166" s="36"/>
-      <c r="F166" s="36"/>
-      <c r="G166" s="36"/>
-      <c r="H166" s="36"/>
-    </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="2" t="s">
+      <c r="B168" s="36"/>
+      <c r="C168" s="37"/>
+      <c r="D168" s="36"/>
+      <c r="E168" s="36"/>
+      <c r="F168" s="36"/>
+      <c r="G168" s="36"/>
+      <c r="H168" s="36"/>
+    </row>
+    <row r="169" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B167" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C167" s="19"/>
-      <c r="D167" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E167" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F167" s="5">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B168" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C168" s="19"/>
-      <c r="D168" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E168" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F168" s="5">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A169" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="B169" s="29" t="s">
         <v>36</v>
@@ -2427,15 +2440,12 @@
         <v>0</v>
       </c>
       <c r="F169" s="5">
-        <v>400</v>
-      </c>
-      <c r="H169" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>36</v>
@@ -2448,15 +2458,12 @@
         <v>0</v>
       </c>
       <c r="F170" s="5">
-        <v>0</v>
-      </c>
-      <c r="H170" s="26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>36</v>
@@ -2469,103 +2476,106 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="25"/>
-      <c r="C172" s="27"/>
-    </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="25"/>
-      <c r="C173" s="27"/>
-    </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B172" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E172" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F172" s="5">
+        <v>0</v>
+      </c>
+      <c r="H172" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B173" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C173" s="19"/>
+      <c r="D173" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E173" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F173" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B181" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C181" s="19"/>
-      <c r="D181" s="18"/>
-      <c r="E181" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F181" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B182" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C182" s="19"/>
-      <c r="D182" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E182" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F182" s="5">
-        <v>20</v>
-      </c>
+    <row r="181" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="25"/>
+      <c r="C181" s="27"/>
+    </row>
+    <row r="182" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="25"/>
+      <c r="C182" s="27"/>
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="B183" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C183" s="19"/>
-      <c r="D183" s="18" t="s">
-        <v>89</v>
-      </c>
+      <c r="D183" s="18"/>
       <c r="E183" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F183" s="5">
-        <v>60</v>
-      </c>
-      <c r="H183" s="1" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="B184" s="29" t="s">
         <v>36</v>
@@ -2578,12 +2588,12 @@
         <v>0</v>
       </c>
       <c r="F184" s="5">
-        <v>78</v>
+        <v>20</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="B185" s="29" t="s">
         <v>36</v>
@@ -2596,12 +2606,15 @@
         <v>0</v>
       </c>
       <c r="F185" s="5">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="B186" s="29" t="s">
         <v>36</v>
@@ -2614,12 +2627,12 @@
         <v>0</v>
       </c>
       <c r="F186" s="5">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B187" s="29" t="s">
         <v>36</v>
@@ -2632,24 +2645,52 @@
         <v>0</v>
       </c>
       <c r="F187" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B188" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C188" s="19"/>
+      <c r="D188" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E188" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B189" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C189" s="19"/>
+      <c r="D189" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E189" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F189" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="25"/>
-      <c r="C188" s="27"/>
-    </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="190" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="25"/>
+      <c r="C190" s="27"/>
+    </row>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="25"/>
-      <c r="C192" s="27"/>
-    </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="25"/>
-      <c r="C193" s="27"/>
-    </row>
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
@@ -2694,511 +2735,479 @@
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="2" t="s">
+    <row r="205" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A205" s="25"/>
+      <c r="C205" s="27"/>
+    </row>
+    <row r="206" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="25"/>
+      <c r="C206" s="27"/>
+    </row>
+    <row r="207" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C205" s="1"/>
-      <c r="E205" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F205" s="24">
-        <v>100000</v>
-      </c>
-      <c r="H205" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C206" s="1"/>
-      <c r="E206" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F206" s="5">
-        <v>1</v>
-      </c>
-      <c r="H206" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A207" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F207" s="5">
+      <c r="F207" s="24">
+        <v>100000</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C208" s="1"/>
+      <c r="E208" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F208" s="5">
+        <v>1</v>
+      </c>
+      <c r="H208" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A209" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C209" s="1"/>
+      <c r="E209" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F209" s="5">
         <v>1500</v>
       </c>
-      <c r="H207" s="1" t="s">
+      <c r="H209" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A209" s="25"/>
-      <c r="C209" s="27"/>
-    </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="25"/>
-      <c r="C210" s="27"/>
-    </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:8" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A224" s="9"/>
-      <c r="C224" s="14"/>
-    </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A225" s="39" t="s">
+    <row r="224" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A224" s="25"/>
+      <c r="C224" s="27"/>
+    </row>
+    <row r="225" spans="1:8" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A225" s="25"/>
+      <c r="C225" s="27"/>
+    </row>
+    <row r="226" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A226" s="9"/>
+      <c r="C226" s="14"/>
+    </row>
+    <row r="227" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A227" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="B225" s="43" t="s">
+      <c r="B227" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C225" s="39" t="s">
+      <c r="C227" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="D225" s="44" t="s">
+      <c r="D227" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="E225" s="43" t="s">
+      <c r="E227" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F225" s="39" t="s">
+      <c r="F227" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="G225" s="39" t="s">
+      <c r="G227" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="H225" s="40"/>
-    </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="2" t="s">
+      <c r="H227" s="40"/>
+    </row>
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A228" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B226" s="6" t="s">
+      <c r="B228" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C226" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D226" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E226" s="6" t="s">
+      <c r="C228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E228" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F226" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G226" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A227" s="47" t="s">
+      <c r="F228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G228" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A229" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B227" s="6" t="s">
+      <c r="B229" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C227" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D227" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E227" s="6" t="s">
+      <c r="C229" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D229" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E229" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F227" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G227" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="47"/>
-      <c r="B228" s="6" t="s">
+      <c r="F229" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G229" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A230" s="49"/>
+      <c r="B230" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C228" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D228" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E228" s="6" t="s">
+      <c r="C230" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D230" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E230" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F228" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G228" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A229" s="47"/>
-      <c r="B229" s="6" t="s">
+      <c r="F230" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G230" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A231" s="49"/>
+      <c r="B231" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C229" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D229" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E229" s="6" t="s">
+      <c r="C231" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D231" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E231" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F229" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G229" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A230" s="47"/>
-      <c r="B230" s="6" t="s">
+      <c r="F231" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G231" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A232" s="49"/>
+      <c r="B232" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C230" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D230" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E230" s="6" t="s">
+      <c r="C232" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F230" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G230" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A231" s="47"/>
-      <c r="B231" s="6" t="s">
+      <c r="F232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G232" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="49"/>
+      <c r="B233" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C231" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D231" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E231" s="6" t="s">
+      <c r="C233" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D233" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E233" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F231" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G231" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A232" s="47"/>
-      <c r="B232" s="6" t="s">
+      <c r="F233" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G233" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A234" s="49"/>
+      <c r="B234" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
+      <c r="C234" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D234" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E234" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G232" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="47"/>
-      <c r="B233" s="6" t="s">
+      <c r="F234" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G234" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A235" s="49"/>
+      <c r="B235" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C233" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D233" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E233" s="6" t="s">
+      <c r="C235" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D235" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E235" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F233" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G233" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="47"/>
-      <c r="B234" s="6" t="s">
+      <c r="F235" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G235" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A236" s="49"/>
+      <c r="B236" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C234" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D234" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E234" s="6" t="s">
+      <c r="C236" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D236" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E236" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F234" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G234" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A235" s="47"/>
-      <c r="B235" s="6" t="s">
+      <c r="F236" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G236" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A237" s="49"/>
+      <c r="B237" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C235" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D235" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E235" s="6" t="s">
+      <c r="C237" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D237" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E237" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F235" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G235" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A236" s="47"/>
-      <c r="B236" s="6" t="s">
+      <c r="F237" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G237" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A238" s="49"/>
+      <c r="B238" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C236" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D236" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E236" s="6" t="s">
+      <c r="C238" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D238" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E238" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F236" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G236" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="47"/>
-      <c r="B237" s="6" t="s">
+      <c r="F238" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G238" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A239" s="49"/>
+      <c r="B239" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C237" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D237" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E237" s="6" t="s">
+      <c r="C239" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D239" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E239" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F237" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G237" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="47"/>
-      <c r="B238" s="6" t="s">
+      <c r="F239" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G239" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A240" s="49"/>
+      <c r="B240" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C238" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D238" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E238" s="6" t="s">
+      <c r="C240" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D240" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E240" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F238" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G238" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="47"/>
-      <c r="B239" s="6" t="s">
+      <c r="F240" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G240" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A241" s="49"/>
+      <c r="B241" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C239" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D239" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E239" s="6" t="s">
+      <c r="C241" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D241" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E241" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F239" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G239" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A240" s="47"/>
-      <c r="B240" s="6" t="s">
+      <c r="F241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G241" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A242" s="49"/>
+      <c r="B242" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C240" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D240" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E240" s="6" t="s">
+      <c r="C242" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D242" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E242" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F240" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G240" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A241" s="47"/>
-      <c r="B241" s="6" t="s">
+      <c r="F242" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G242" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A243" s="49"/>
+      <c r="B243" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C241" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D241" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E241" s="6" t="s">
+      <c r="C243" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D243" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E243" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="F241" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G241" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B242" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C242" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D242" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E242" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F242" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G242" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B243" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C243" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D243" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E243" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="F243" s="4" t="b">
         <v>1</v>
@@ -3209,98 +3218,130 @@
     </row>
     <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B244" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C244" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D244" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E244" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F244" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G244" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B245" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C245" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D245" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E245" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F245" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G245" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B246" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C244" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D244" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E244" s="6" t="s">
+      <c r="C246" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D246" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E246" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F244" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G244" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A245" s="50" t="s">
+      <c r="F246" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G246" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="B245" s="6" t="s">
+      <c r="B247" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C245" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D245" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E245" s="6" t="s">
+      <c r="C247" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D247" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E247" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F245" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G245" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A246" s="50"/>
-      <c r="B246" s="6" t="s">
+      <c r="F247" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G247" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A248" s="52"/>
+      <c r="B248" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C246" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D246" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E246" s="6" t="s">
+      <c r="C248" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D248" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E248" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F246" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G246" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H246" s="1" t="s">
+      <c r="F248" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G248" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H248" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B247" s="6" t="s">
+    <row r="249" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B249" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C247" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D247" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E247" s="6" t="s">
+      <c r="C249" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D249" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E249" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F247" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G247" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A248" s="25"/>
-      <c r="C248" s="27"/>
-    </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="25"/>
-      <c r="C249" s="27"/>
+      <c r="F249" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G249" s="4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="25"/>
@@ -3386,55 +3427,38 @@
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A274" s="35" t="s">
+    <row r="273" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A273" s="25"/>
+      <c r="C273" s="27"/>
+    </row>
+    <row r="274" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A274" s="25"/>
+      <c r="C274" s="27"/>
+    </row>
+    <row r="275" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A276" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B274" s="36"/>
-      <c r="C274" s="37"/>
-      <c r="D274" s="36"/>
-      <c r="E274" s="36"/>
-      <c r="F274" s="36"/>
-      <c r="G274" s="36"/>
-      <c r="H274" s="36"/>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A275" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B275" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C275" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A276" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B276" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C276" s="5">
-        <v>1</v>
-      </c>
-      <c r="H276" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="B276" s="36"/>
+      <c r="C276" s="37"/>
+      <c r="D276" s="36"/>
+      <c r="E276" s="36"/>
+      <c r="F276" s="36"/>
+      <c r="G276" s="36"/>
+      <c r="H276" s="36"/>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B277" s="28" t="s">
         <v>76</v>
@@ -3442,13 +3466,10 @@
       <c r="C277" s="5">
         <v>1</v>
       </c>
-      <c r="H277" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B278" s="28" t="s">
         <v>76</v>
@@ -3456,193 +3477,221 @@
       <c r="C278" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+      <c r="H278" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A279" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B279" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C279" s="5">
+        <v>1</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A280" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B280" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C280" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A302" s="9"/>
-      <c r="C302" s="14"/>
-    </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A304" s="39" t="s">
+    <row r="289" spans="1:3" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="303" spans="1:3" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="9"/>
+      <c r="C304" s="14"/>
+    </row>
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="306" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A306" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B304" s="40"/>
-      <c r="C304" s="42"/>
-      <c r="D304" s="40"/>
-      <c r="E304" s="40"/>
-      <c r="F304" s="40"/>
-      <c r="G304" s="40"/>
-      <c r="H304" s="40"/>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A305" s="2" t="s">
+      <c r="B306" s="40"/>
+      <c r="C306" s="42"/>
+      <c r="D306" s="40"/>
+      <c r="E306" s="40"/>
+      <c r="F306" s="40"/>
+      <c r="G306" s="40"/>
+      <c r="H306" s="40"/>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A307" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C305" s="31" t="s">
+      <c r="C307" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B306" s="22" t="s">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B308" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C306" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B307" s="22" t="s">
+      <c r="C308" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B309" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C307" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B308" s="22" t="s">
+      <c r="C309" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B310" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C308" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B309" s="22" t="s">
+      <c r="C310" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B311" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C309" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B310" s="22" t="s">
+      <c r="C311" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B312" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C310" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B311" s="22" t="s">
+      <c r="C312" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B313" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C311" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B312" s="22" t="s">
+      <c r="C313" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B314" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C312" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B313" s="22" t="s">
+      <c r="C314" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B315" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C313" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B314" s="22" t="s">
+      <c r="C315" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B316" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C314" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B315" s="22" t="s">
+      <c r="C316" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B317" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C315" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B316" s="22" t="s">
+      <c r="C317" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B318" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C316" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B317" s="22" t="s">
+      <c r="C318" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B319" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C317" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B318" s="22" t="s">
+      <c r="C319" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B320" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C318" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B319" s="22" t="s">
+      <c r="C320" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B321" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C319" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B320" s="22" t="s">
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B322" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C320" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A325" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F330" s="2"/>
+      <c r="C322" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A327" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F332" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B6:H6"/>
-    <mergeCell ref="A227:A241"/>
+    <mergeCell ref="A229:A243"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B4:H4"/>
-    <mergeCell ref="A245:A246"/>
+    <mergeCell ref="A247:A248"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C306:C320 C35:C36">
+  <conditionalFormatting sqref="C228:D249 F228:G249 C79 C308:C322 C35:C36">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
@@ -3669,14 +3718,14 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F170 F183:F189 F173" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C279" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C280" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C37" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F171" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F169:F173" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
@@ -3688,22 +3737,22 @@
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169:F170" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F206" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F207" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F171:F172" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F207" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F208" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F209" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F102" xr:uid="{C22C312A-4C0D-465E-AA40-04829D4E1DD5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F103" xr:uid="{70E3A2FC-178F-4589-82CF-31382B011A9B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C136" xr:uid="{DCD0DDF5-CAA3-4B00-8005-5B7C31C37DA9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand input file" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="C126" xr:uid="{C0A91F47-4A7A-4D7C-8BF7-42344234CEB1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand default value" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="F126" xr:uid="{0207F56E-8010-40B0-B53E-04E2603C9864}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F164" xr:uid="{9C9B8F4F-043F-41E7-8848-A40DCB72B3F5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F163" xr:uid="{C47BA5BE-2C24-4654-BEF9-EA5B433BE488}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F166" xr:uid="{9C9B8F4F-043F-41E7-8848-A40DCB72B3F5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F165" xr:uid="{C47BA5BE-2C24-4654-BEF9-EA5B433BE488}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F172" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F172" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C172" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C164" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C163" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{F5C6CB55-A203-47FE-96B0-DC9C451014C9}"/>
   </dataValidations>
@@ -3716,7 +3765,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C306:C320 F226:G247 C226:D247</xm:sqref>
+          <xm:sqref>C308:C322 F228:G249 C228:D249</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Corrections in preprocessing in order to allow simulation if PtL Demand is empty in ConfigFile Update cost of Unserved H2 in ConfigFile
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979EB48C-7A96-4A23-B6C7-90592591B5B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35F331B-9155-462F-B91D-89436D55EE2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,9 +692,6 @@
     <t>H2 flexible capacities</t>
   </si>
   <si>
-    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities.csv</t>
-  </si>
-  <si>
     <t>Can remain empty if no flexible part of the H2 demand</t>
   </si>
   <si>
@@ -702,6 +699,9 @@
   </si>
   <si>
     <t>Dispa-SET Configuration File (v20.02)</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/PtL_Capacities.csv</t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1411,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="F182" sqref="F182"/>
+    <sheetView tabSelected="1" topLeftCell="C134" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1430,7 +1430,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2341,7 +2341,7 @@
         <v>217</v>
       </c>
       <c r="H160" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2352,10 +2352,10 @@
         <v>36</v>
       </c>
       <c r="C161" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="H161" s="26" t="s">
         <v>219</v>
-      </c>
-      <c r="H161" s="26" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="F173" s="5">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="174" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -3676,7 +3676,7 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
correct typo in Config and correct error in PtL demand
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35F331B-9155-462F-B91D-89436D55EE2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B8016-58BF-4BD7-9557-27B0FF325EE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,7 +701,7 @@
     <t>Dispa-SET Configuration File (v20.02)</t>
   </si>
   <si>
-    <t>Database/NearZeroCarbon/H2_demand/PtL_Capacities.csv</t>
+    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities.csv</t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1411,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C134" workbookViewId="0">
-      <selection activeCell="C171" sqref="C171"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1732,7 +1732,7 @@
         <v>38</v>
       </c>
       <c r="C58" s="17">
-        <v>42735</v>
+        <v>42400</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Last modifs of Database
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B8016-58BF-4BD7-9557-27B0FF325EE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA31E0D3-4C6B-4612-8E73-F5E437BCF82F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,12 +683,6 @@
     <t>H2 flexible demand</t>
   </si>
   <si>
-    <t>Database/NearZeroCarbon/H2_demand/H2_rigid_Demand_2050.csv</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/H2_demand/H2_PtL_Demand_2050.csv</t>
-  </si>
-  <si>
     <t>H2 flexible capacities</t>
   </si>
   <si>
@@ -701,7 +695,13 @@
     <t>Dispa-SET Configuration File (v20.02)</t>
   </si>
   <si>
-    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities.csv</t>
+    <t>Database/NearZeroCarbon/H2_demand/H2_rigid_Demand_2050_ALLFLEX.csv</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/H2_PtL_Demand_2050_ALLFLEX.csv</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities_2050_ALLFLEX.csv</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1411,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
       <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1430,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -1732,7 +1732,7 @@
         <v>38</v>
       </c>
       <c r="C58" s="17">
-        <v>42400</v>
+        <v>42735</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>72</v>
@@ -2236,7 +2236,7 @@
         <v>36</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>89</v>
@@ -2338,15 +2338,15 @@
         <v>36</v>
       </c>
       <c r="C160" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="H160" s="26" t="s">
         <v>217</v>
-      </c>
-      <c r="H160" s="26" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B161" s="46" t="s">
         <v>36</v>
@@ -2355,7 +2355,7 @@
         <v>222</v>
       </c>
       <c r="H161" s="26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3676,7 +3676,7 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Clean-up of the previous commits
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
+++ b/ConfigFiles/Config_NearZeroCarbon_ALLFLEX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\AppData\Local\Temp\Mxt201\RemoteFiles\1574982_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA31E0D3-4C6B-4612-8E73-F5E437BCF82F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1F8E8-51E5-448C-B19F-AD7FA778EED3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,37 +671,37 @@
     <t>Configuration file for paper storage. Simulation time is 1 year.</t>
   </si>
   <si>
+    <t>Database/NearZeroCarbon/DayAheadNTC/1h/NTC_2050.csv</t>
+  </si>
+  <si>
+    <t>H2 rigid Demand</t>
+  </si>
+  <si>
+    <t>H2 flexible demand</t>
+  </si>
+  <si>
+    <t>H2 flexible capacities</t>
+  </si>
+  <si>
+    <t>Can remain empty if no flexible part of the H2 demand</t>
+  </si>
+  <si>
+    <t>End of the Config file. This must be line number 327!</t>
+  </si>
+  <si>
+    <t>Dispa-SET Configuration File (v20.02)</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/H2_rigid_Demand_2050_ALLFLEX.csv</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/H2_PtL_Demand_2050_ALLFLEX.csv</t>
+  </si>
+  <si>
+    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities_2050_ALLFLEX.csv</t>
+  </si>
+  <si>
     <t>Simulations/JRC_EU_TIMES/NearZeroCarbon/ALLFLEX</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/DayAheadNTC/1h/NTC_2050.csv</t>
-  </si>
-  <si>
-    <t>H2 rigid Demand</t>
-  </si>
-  <si>
-    <t>H2 flexible demand</t>
-  </si>
-  <si>
-    <t>H2 flexible capacities</t>
-  </si>
-  <si>
-    <t>Can remain empty if no flexible part of the H2 demand</t>
-  </si>
-  <si>
-    <t>End of the Config file. This must be line number 327!</t>
-  </si>
-  <si>
-    <t>Dispa-SET Configuration File (v20.02)</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/H2_demand/H2_rigid_Demand_2050_ALLFLEX.csv</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/H2_demand/H2_PtL_Demand_2050_ALLFLEX.csv</t>
-  </si>
-  <si>
-    <t>Database/NearZeroCarbon/H2_demand/PtL_capacities_2050_ALLFLEX.csv</t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1411,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="F173" sqref="F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1430,7 +1430,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -1623,7 +1623,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -2146,7 +2146,7 @@
         <v>36</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>89</v>
@@ -2230,13 +2230,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>89</v>
@@ -2332,30 +2332,30 @@
     </row>
     <row r="160" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B160" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C160" s="47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H160" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B161" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C161" s="47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H161" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2440,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="F169" s="5">
-        <v>350</v>
+        <v>200</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2458,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="F170" s="5">
-        <v>175</v>
+        <v>300</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>178</v>
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="F173" s="5">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="174" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -3676,7 +3676,7 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>